<commit_message>
fix rename and excel sample
</commit_message>
<xml_diff>
--- a/public/files/Spots.xlsx
+++ b/public/files/Spots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\both9\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7107C6CF-533A-4C3F-9959-02938837E7C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3069F5-4D19-4FF8-AAF8-535C2E13E862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="70">
   <si>
     <t>TEST2</t>
   </si>
@@ -149,10 +149,6 @@
   </si>
   <si>
     <t>通勤時間</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>預計停留時間</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -345,10 +341,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>半天以上</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">JPY 3,600~ / </t>
     </r>
@@ -374,6 +366,10 @@
   </si>
   <si>
     <t>豐洲-東京都江東區豐洲6-1-16 （teamLab Planets TOKYO）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>預計停留時間(hr)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -868,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -918,53 +914,53 @@
         <v>37</v>
       </c>
       <c r="K1" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="L1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="340.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>66</v>
+      <c r="K2" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -993,7 +989,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -1025,7 +1021,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -1051,7 +1047,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -1074,7 +1070,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -1097,7 +1093,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
@@ -1129,7 +1125,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -1161,7 +1157,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -1193,7 +1189,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
@@ -1225,7 +1221,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -1257,7 +1253,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -1289,7 +1285,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -1321,7 +1317,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
@@ -1347,7 +1343,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -1370,7 +1366,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
@@ -1393,7 +1389,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
@@ -1425,7 +1421,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
@@ -1457,7 +1453,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
@@ -1489,7 +1485,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>

</xml_diff>